<commit_message>
leer productos con descuentos
</commit_message>
<xml_diff>
--- a/CODIGOS DE ARTICULOS.xlsx
+++ b/CODIGOS DE ARTICULOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\JAJI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3FB203-6BDC-424A-BC31-3ECF7228A922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ACF125-8797-420B-B63A-3532981B2FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B340ADFB-D82E-4E45-9970-9F12D4CC00F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B340ADFB-D82E-4E45-9970-9F12D4CC00F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -526,8 +526,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.399999999999999" customHeight="1"/>

</xml_diff>